<commit_message>
Improving the Excel template
</commit_message>
<xml_diff>
--- a/templates/WinnersList.xlsx
+++ b/templates/WinnersList.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\turco\source\repos\GalaPresentation\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FACB3D0D-C08F-4692-BA6C-3706D02E2113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890A6710-8787-472F-A7CD-C527C3303FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" tabRatio="839" xr2:uid="{49F4F76C-EBC2-44CC-A8DB-D942F0D743B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Prix 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Prix 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,12 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>Nom</t>
-  </si>
-  <si>
-    <t>Numéro</t>
+    <t>Émile T.</t>
   </si>
 </sst>
 </file>
@@ -441,7 +439,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,8 +448,8 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
+      <c r="B1" s="2">
+        <v>1111</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -588,4 +586,27 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4DD94D-A510-4C6B-84EC-1D223C193EB9}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changing the format of the Excel sheet
All the prizes are now in a single sheet, refer to the template to see how to build one.

Changing the format of the PowerPoint too so it looks cleaner, now the number of people per slide is not continuous anymore, so having a slide with a different number of winners requires changing the slideLayouts array in the code.
</commit_message>
<xml_diff>
--- a/templates/WinnersList.xlsx
+++ b/templates/WinnersList.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\turco\source\repos\GalaPresentation\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890A6710-8787-472F-A7CD-C527C3303FA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D56723-6CDD-4B47-8E41-781B59A07DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" tabRatio="839" xr2:uid="{49F4F76C-EBC2-44CC-A8DB-D942F0D743B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Prix 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Prix 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Worsheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,9 +36,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
-  <si>
-    <t>Émile T.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Prize name</t>
+  </si>
+  <si>
+    <t>Prize category</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>Prize 1</t>
+  </si>
+  <si>
+    <t>Prize 1 nominations</t>
+  </si>
+  <si>
+    <t>Prize 1 winners</t>
   </si>
 </sst>
 </file>
@@ -439,62 +468,108 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>1111</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1111</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.35">
@@ -586,27 +661,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4DD94D-A510-4C6B-84EC-1D223C193EB9}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1111</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>